<commit_message>
EPBDS-13201 Add tests for alternative logic operators
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/LogicOperator.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/LogicOperator.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/demoMaster/openl-demo/user-workspace4/DEFAULT/LogicOperator/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{561AC5DB-BBD6-2A4D-9DCA-ED61817C5B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="34840" windowHeight="20360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Not" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="66">
   <si>
     <t>C1</t>
   </si>
@@ -176,12 +182,51 @@
   </si>
   <si>
     <t>Test notMore</t>
+  </si>
+  <si>
+    <t>// Alternative</t>
+  </si>
+  <si>
+    <t>Rules String notMoreAlt (int v1, int v2)</t>
+  </si>
+  <si>
+    <t>Test notMoreAlt</t>
+  </si>
+  <si>
+    <t>!(v1 &gt; v2)</t>
+  </si>
+  <si>
+    <t>Method Boolean InverseAlt (Boolean in)</t>
+  </si>
+  <si>
+    <t>return !in;</t>
+  </si>
+  <si>
+    <t>Test InverseAlt</t>
+  </si>
+  <si>
+    <t>Method Boolean DisjunctionAlt (Boolean a, Boolean b)</t>
+  </si>
+  <si>
+    <t>return a || b;</t>
+  </si>
+  <si>
+    <t>Test DisjunctionAlt</t>
+  </si>
+  <si>
+    <t>Method Boolean ConjunctionAlt (Boolean a, Boolean b)</t>
+  </si>
+  <si>
+    <t>Test ConjunctionAlt</t>
+  </si>
+  <si>
+    <t>return a &amp;&amp; b;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -256,17 +301,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -328,7 +372,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,9 +405,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -396,6 +457,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -571,40 +649,40 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B6:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="42.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="38.1640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42.33203125" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="28" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="50.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="50.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
@@ -615,7 +693,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
@@ -626,7 +704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="b">
         <v>1</v>
       </c>
@@ -637,7 +715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="b">
         <v>0</v>
       </c>
@@ -648,16 +726,90 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -665,177 +817,337 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B6:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD20"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="47.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="C12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="C14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="C15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="C18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -843,323 +1155,614 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:E20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B6:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="C12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="C13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="C14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="C15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="C16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="C18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E34" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E35" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E37" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:D19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B6:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="8" t="s">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="4">
         <v>2</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="4">
         <v>3</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
         <v>11</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>11</v>
       </c>
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="4" t="s">
         <v>7</v>
       </c>
     </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="4">
+        <v>2</v>
+      </c>
+      <c r="C36" s="4">
+        <v>3</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="1">
+        <v>11</v>
+      </c>
+      <c r="C37" s="1">
+        <v>11</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B32:D32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>